<commit_message>
The program now works with all surveys later than 1022
This applies to both FindRemovable and totalActivity.
</commit_message>
<xml_diff>
--- a/Output/QC-Removable.xlsx
+++ b/Output/QC-Removable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>File Name</t>
   </si>
@@ -32,45 +32,12 @@
   </si>
   <si>
     <t>Cal DueDate</t>
-  </si>
-  <si>
-    <t>Characterization 011020-950.xlsx</t>
-  </si>
-  <si>
-    <t>Survey Sheet (2)</t>
-  </si>
-  <si>
-    <t>INIS-011020-950</t>
-  </si>
-  <si>
-    <t>3030</t>
-  </si>
-  <si>
-    <t>247862</t>
-  </si>
-  <si>
-    <t>Characterization 012320-1045.xlsx</t>
-  </si>
-  <si>
-    <t>Scan and Data</t>
-  </si>
-  <si>
-    <t>INIS-012320-1045</t>
-  </si>
-  <si>
-    <t>2929/43-10-1</t>
-  </si>
-  <si>
-    <t>208310/PR229222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -100,9 +67,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,46 +389,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43865</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44141</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>